<commit_message>
change way of data_import model, busy on date-based indexing
</commit_message>
<xml_diff>
--- a/src/silk_basket/example/data/GDP.xlsx
+++ b/src/silk_basket/example/data/GDP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\scrt_projs\silk_peg\src\silk_peg\example\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\scrt_projs\silk_basket\src\silk_basket\example\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B2B8D21-F473-41F5-A7B6-D25E9E06E296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A81390-0F5C-4022-9B58-745B198E2BE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{53F89C0F-D25F-4D88-BF3A-84C5F376C676}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{53F89C0F-D25F-4D88-BF3A-84C5F376C676}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="19">
   <si>
     <t>time</t>
   </si>
@@ -82,9 +82,6 @@
   </si>
   <si>
     <t>Singapore</t>
-  </si>
-  <si>
-    <t>Total</t>
   </si>
   <si>
     <t xml:space="preserve"> NaN </t>
@@ -138,18 +135,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -165,7 +160,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -453,7 +448,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -461,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DABA2002-F806-42C6-BFDD-E3D4A0EB42EF}">
-  <dimension ref="A1:S63"/>
+  <dimension ref="A1:R62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="Q63" sqref="Q63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,7 +468,7 @@
     <col min="18" max="18" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -508,13 +503,13 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M1" t="s">
         <v>11</v>
       </c>
       <c r="N1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O1" t="s">
         <v>12</v>
@@ -528,11 +523,8 @@
       <c r="R1" t="s">
         <v>15</v>
       </c>
-      <c r="S1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>22250</v>
       </c>
@@ -561,7 +553,7 @@
         <v>3.96</v>
       </c>
       <c r="J2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K2">
         <v>15.17</v>
@@ -570,7 +562,7 @@
         <v>18.600000000000001</v>
       </c>
       <c r="M2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N2">
         <v>9.52</v>
@@ -587,12 +579,8 @@
       <c r="R2">
         <v>0.7</v>
       </c>
-      <c r="S2" s="2">
-        <f t="shared" ref="S2:S63" si="0">SUM(B2:R2)</f>
-        <v>1125.8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>22615</v>
       </c>
@@ -621,7 +609,7 @@
         <v>2.42</v>
       </c>
       <c r="J3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K3">
         <v>15.24</v>
@@ -630,7 +618,7 @@
         <v>19.7</v>
       </c>
       <c r="M3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N3">
         <v>10.71</v>
@@ -647,12 +635,8 @@
       <c r="R3">
         <v>0.76</v>
       </c>
-      <c r="S3" s="2">
-        <f t="shared" si="0"/>
-        <v>1173.3800000000003</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>22980</v>
       </c>
@@ -681,7 +665,7 @@
         <v>2.81</v>
       </c>
       <c r="J4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K4">
         <v>19.93</v>
@@ -690,7 +674,7 @@
         <v>19.899999999999999</v>
       </c>
       <c r="M4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N4">
         <v>11.88</v>
@@ -707,12 +691,8 @@
       <c r="R4">
         <v>0.83</v>
       </c>
-      <c r="S4" s="2">
-        <f t="shared" si="0"/>
-        <v>1266.4900000000005</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>23345</v>
       </c>
@@ -741,7 +721,7 @@
         <v>3.99</v>
       </c>
       <c r="J5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K5">
         <v>23.02</v>
@@ -750,7 +730,7 @@
         <v>21.5</v>
       </c>
       <c r="M5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N5">
         <v>13.06</v>
@@ -767,12 +747,8 @@
       <c r="R5">
         <v>0.92</v>
       </c>
-      <c r="S5" s="2">
-        <f t="shared" si="0"/>
-        <v>1373.71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>23711</v>
       </c>
@@ -801,7 +777,7 @@
         <v>3.46</v>
       </c>
       <c r="J6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K6">
         <v>21.21</v>
@@ -810,7 +786,7 @@
         <v>23.8</v>
       </c>
       <c r="M6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N6">
         <v>14.48</v>
@@ -827,12 +803,8 @@
       <c r="R6">
         <v>0.89</v>
       </c>
-      <c r="S6" s="2">
-        <f t="shared" si="0"/>
-        <v>1505.2500000000005</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>24076</v>
       </c>
@@ -861,7 +833,7 @@
         <v>3.12</v>
       </c>
       <c r="J7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K7">
         <v>21.79</v>
@@ -870,7 +842,7 @@
         <v>25.9</v>
       </c>
       <c r="M7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N7">
         <v>15.35</v>
@@ -887,12 +859,8 @@
       <c r="R7">
         <v>0.97</v>
       </c>
-      <c r="S7" s="2">
-        <f t="shared" si="0"/>
-        <v>1640.6599999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>24441</v>
       </c>
@@ -921,7 +889,7 @@
         <v>3.93</v>
       </c>
       <c r="J8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K8">
         <v>27.06</v>
@@ -930,7 +898,7 @@
         <v>27.3</v>
       </c>
       <c r="M8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N8">
         <v>16.48</v>
@@ -947,12 +915,8 @@
       <c r="R8">
         <v>1.1000000000000001</v>
       </c>
-      <c r="S8" s="2">
-        <f t="shared" si="0"/>
-        <v>1783.3799999999997</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>24806</v>
       </c>
@@ -981,7 +945,7 @@
         <v>4.8600000000000003</v>
       </c>
       <c r="J9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K9">
         <v>30.59</v>
@@ -1007,12 +971,8 @@
       <c r="R9">
         <v>1.24</v>
       </c>
-      <c r="S9" s="2">
-        <f t="shared" si="0"/>
-        <v>1915.6100000000004</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>25172</v>
       </c>
@@ -1041,7 +1001,7 @@
         <v>6.12</v>
       </c>
       <c r="J10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K10">
         <v>33.880000000000003</v>
@@ -1067,12 +1027,8 @@
       <c r="R10">
         <v>1.43</v>
       </c>
-      <c r="S10" s="2">
-        <f t="shared" si="0"/>
-        <v>2070.4799999999996</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>25537</v>
       </c>
@@ -1101,7 +1057,7 @@
         <v>7.68</v>
       </c>
       <c r="J11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K11">
         <v>37.46</v>
@@ -1127,12 +1083,8 @@
       <c r="R11">
         <v>1.66</v>
       </c>
-      <c r="S11" s="2">
-        <f t="shared" si="0"/>
-        <v>2281.7099999999991</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>25902</v>
       </c>
@@ -1161,7 +1113,7 @@
         <v>9.01</v>
       </c>
       <c r="J12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K12">
         <v>42.33</v>
@@ -1187,12 +1139,8 @@
       <c r="R12">
         <v>1.92</v>
       </c>
-      <c r="S12" s="2">
-        <f t="shared" si="0"/>
-        <v>2498.1400000000008</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>26267</v>
       </c>
@@ -1221,7 +1169,7 @@
         <v>9.9</v>
       </c>
       <c r="J13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K13">
         <v>49.2</v>
@@ -1247,12 +1195,8 @@
       <c r="R13">
         <v>2.2599999999999998</v>
       </c>
-      <c r="S13" s="2">
-        <f t="shared" si="0"/>
-        <v>2765.4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>26633</v>
       </c>
@@ -1281,7 +1225,7 @@
         <v>10.86</v>
       </c>
       <c r="J14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K14">
         <v>58.54</v>
@@ -1307,12 +1251,8 @@
       <c r="R14">
         <v>2.72</v>
       </c>
-      <c r="S14" s="2">
-        <f t="shared" si="0"/>
-        <v>3202.91</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>26998</v>
       </c>
@@ -1341,7 +1281,7 @@
         <v>13.88</v>
       </c>
       <c r="J15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K15">
         <v>79.28</v>
@@ -1367,12 +1307,8 @@
       <c r="R15">
         <v>3.7</v>
       </c>
-      <c r="S15" s="2">
-        <f t="shared" si="0"/>
-        <v>3880.31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>27363</v>
       </c>
@@ -1401,7 +1337,7 @@
         <v>19.54</v>
       </c>
       <c r="J16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K16">
         <v>105.14</v>
@@ -1427,12 +1363,8 @@
       <c r="R16">
         <v>5.22</v>
       </c>
-      <c r="S16" s="2">
-        <f t="shared" si="0"/>
-        <v>4359.3100000000004</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>27728</v>
       </c>
@@ -1461,7 +1393,7 @@
         <v>21.78</v>
       </c>
       <c r="J17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K17">
         <v>123.71</v>
@@ -1487,12 +1419,8 @@
       <c r="R17">
         <v>5.63</v>
       </c>
-      <c r="S17" s="2">
-        <f t="shared" si="0"/>
-        <v>4888.79</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>28094</v>
       </c>
@@ -1521,7 +1449,7 @@
         <v>29.9</v>
       </c>
       <c r="J18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K18">
         <v>152.68</v>
@@ -1547,12 +1475,8 @@
       <c r="R18">
         <v>6.33</v>
       </c>
-      <c r="S18" s="2">
-        <f t="shared" si="0"/>
-        <v>5297.1899999999987</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>28459</v>
       </c>
@@ -1581,7 +1505,7 @@
         <v>38.450000000000003</v>
       </c>
       <c r="J19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K19">
         <v>176.17</v>
@@ -1607,12 +1531,8 @@
       <c r="R19">
         <v>6.62</v>
       </c>
-      <c r="S19" s="2">
-        <f t="shared" si="0"/>
-        <v>6000.39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>28824</v>
       </c>
@@ -1641,7 +1561,7 @@
         <v>51.97</v>
       </c>
       <c r="J20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K20">
         <v>200.8</v>
@@ -1667,12 +1587,8 @@
       <c r="R20">
         <v>7.52</v>
       </c>
-      <c r="S20" s="2">
-        <f t="shared" si="0"/>
-        <v>7135.55</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>29189</v>
       </c>
@@ -1701,7 +1617,7 @@
         <v>66.95</v>
       </c>
       <c r="J21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K21">
         <v>224.97</v>
@@ -1727,12 +1643,8 @@
       <c r="R21">
         <v>9.3000000000000007</v>
       </c>
-      <c r="S21" s="2">
-        <f t="shared" si="0"/>
-        <v>8205.57</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>29555</v>
       </c>
@@ -1761,7 +1673,7 @@
         <v>65.400000000000006</v>
       </c>
       <c r="J22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K22">
         <v>235.02</v>
@@ -1787,12 +1699,8 @@
       <c r="R22">
         <v>11.9</v>
       </c>
-      <c r="S22" s="2">
-        <f t="shared" si="0"/>
-        <v>9073.9500000000007</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>29920</v>
       </c>
@@ -1821,7 +1729,7 @@
         <v>72.930000000000007</v>
       </c>
       <c r="J23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K23">
         <v>263.56</v>
@@ -1847,12 +1755,8 @@
       <c r="R23">
         <v>14.18</v>
       </c>
-      <c r="S23" s="2">
-        <f t="shared" si="0"/>
-        <v>9226.380000000001</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>30285</v>
       </c>
@@ -1881,7 +1785,7 @@
         <v>78.36</v>
       </c>
       <c r="J24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K24">
         <v>281.68</v>
@@ -1907,12 +1811,8 @@
       <c r="R24">
         <v>16.079999999999998</v>
       </c>
-      <c r="S24" s="2">
-        <f t="shared" si="0"/>
-        <v>9222.1399999999976</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>30650</v>
       </c>
@@ -1941,7 +1841,7 @@
         <v>87.76</v>
       </c>
       <c r="J25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K25">
         <v>203.3</v>
@@ -1967,12 +1867,8 @@
       <c r="R25">
         <v>17.78</v>
       </c>
-      <c r="S25" s="2">
-        <f t="shared" si="0"/>
-        <v>9498.1899999999969</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>31016</v>
       </c>
@@ -2001,7 +1897,7 @@
         <v>97.51</v>
       </c>
       <c r="J26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K26">
         <v>209.02</v>
@@ -2027,12 +1923,8 @@
       <c r="R26">
         <v>19.75</v>
       </c>
-      <c r="S26" s="2">
-        <f t="shared" si="0"/>
-        <v>9922.6500000000033</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>31381</v>
       </c>
@@ -2061,7 +1953,7 @@
         <v>101.3</v>
       </c>
       <c r="J27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K27">
         <v>222.94</v>
@@ -2087,12 +1979,8 @@
       <c r="R27">
         <v>19.16</v>
       </c>
-      <c r="S27" s="2">
-        <f t="shared" si="0"/>
-        <v>10496.990000000002</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>31746</v>
       </c>
@@ -2121,7 +2009,7 @@
         <v>116.84</v>
       </c>
       <c r="J28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K28">
         <v>268.14</v>
@@ -2147,12 +2035,8 @@
       <c r="R28">
         <v>18.59</v>
       </c>
-      <c r="S28" s="2">
-        <f t="shared" si="0"/>
-        <v>12680.02</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>32111</v>
       </c>
@@ -2181,7 +2065,7 @@
         <v>147.94999999999999</v>
       </c>
       <c r="J29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K29">
         <v>294.08</v>
@@ -2207,12 +2091,8 @@
       <c r="R29">
         <v>20.92</v>
       </c>
-      <c r="S29" s="2">
-        <f t="shared" si="0"/>
-        <v>14568.02</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>32477</v>
       </c>
@@ -2267,12 +2147,8 @@
       <c r="R30">
         <v>25.37</v>
       </c>
-      <c r="S30" s="2">
-        <f t="shared" si="0"/>
-        <v>16954.91</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>32842</v>
       </c>
@@ -2327,12 +2203,8 @@
       <c r="R31">
         <v>30.47</v>
       </c>
-      <c r="S31" s="2">
-        <f t="shared" si="0"/>
-        <v>17744.53</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>33207</v>
       </c>
@@ -2387,12 +2259,8 @@
       <c r="R32">
         <v>36.14</v>
       </c>
-      <c r="S32" s="2">
-        <f t="shared" si="0"/>
-        <v>19859.550000000003</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>33572</v>
       </c>
@@ -2447,12 +2315,8 @@
       <c r="R33">
         <v>45.47</v>
       </c>
-      <c r="S33" s="2">
-        <f t="shared" si="0"/>
-        <v>21017.890000000003</v>
-      </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33938</v>
       </c>
@@ -2507,12 +2371,8 @@
       <c r="R34">
         <v>52.13</v>
       </c>
-      <c r="S34" s="2">
-        <f t="shared" si="0"/>
-        <v>22237.739999999998</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34303</v>
       </c>
@@ -2567,69 +2427,65 @@
       <c r="R35">
         <v>60.6</v>
       </c>
-      <c r="S35" s="2">
-        <f t="shared" si="0"/>
-        <v>22430.249999999993</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34668</v>
       </c>
       <c r="B36" s="2">
-        <f t="shared" ref="B36:O36" si="1">AVERAGE(B35,B37)</f>
+        <f t="shared" ref="B36:O36" si="0">AVERAGE(B35,B37)</f>
         <v>7249.1550000000007</v>
       </c>
       <c r="C36" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>589.64</v>
       </c>
       <c r="D36" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6844.7349999999997</v>
       </c>
       <c r="E36" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4999.8500000000004</v>
       </c>
       <c r="F36" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1201.5</v>
       </c>
       <c r="G36" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>319.78999999999996</v>
       </c>
       <c r="H36" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>590.59999999999991</v>
       </c>
       <c r="I36" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>479.625</v>
       </c>
       <c r="J36" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>415.31</v>
       </c>
       <c r="K36" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>603.55499999999995</v>
       </c>
       <c r="L36" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>339.4</v>
       </c>
       <c r="M36" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>180.07</v>
       </c>
       <c r="N36" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>312.8</v>
       </c>
       <c r="O36" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>174.82999999999998</v>
       </c>
       <c r="P36">
@@ -2641,12 +2497,8 @@
       <c r="R36">
         <v>73.69</v>
       </c>
-      <c r="S36" s="2">
-        <f t="shared" si="0"/>
-        <v>24730.710000000003</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35033</v>
       </c>
@@ -2701,12 +2553,8 @@
       <c r="R37">
         <v>87.81</v>
       </c>
-      <c r="S37" s="2">
-        <f t="shared" si="0"/>
-        <v>27072.750000000007</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>35399</v>
       </c>
@@ -2761,12 +2609,8 @@
       <c r="R38">
         <v>96.3</v>
       </c>
-      <c r="S38" s="2">
-        <f t="shared" si="0"/>
-        <v>27456.079999999998</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>35764</v>
       </c>
@@ -2821,12 +2665,8 @@
       <c r="R39">
         <v>100.12</v>
       </c>
-      <c r="S39" s="2">
-        <f t="shared" si="0"/>
-        <v>27135.890000000003</v>
-      </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>36129</v>
       </c>
@@ -2881,12 +2721,8 @@
       <c r="R40">
         <v>85.73</v>
       </c>
-      <c r="S40" s="2">
-        <f t="shared" si="0"/>
-        <v>27149.420000000006</v>
-      </c>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>36494</v>
       </c>
@@ -2941,12 +2777,8 @@
       <c r="R41">
         <v>86.28</v>
       </c>
-      <c r="S41" s="2">
-        <f t="shared" si="0"/>
-        <v>28193.129999999997</v>
-      </c>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>36860</v>
       </c>
@@ -3001,12 +2833,8 @@
       <c r="R42">
         <v>96.07</v>
       </c>
-      <c r="S42" s="2">
-        <f t="shared" si="0"/>
-        <v>28938.83</v>
-      </c>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>37225</v>
       </c>
@@ -3061,12 +2889,8 @@
       <c r="R43">
         <v>89.79</v>
       </c>
-      <c r="S43" s="2">
-        <f t="shared" si="0"/>
-        <v>28697.19</v>
-      </c>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>37590</v>
       </c>
@@ -3121,12 +2945,8 @@
       <c r="R44">
         <v>92.54</v>
       </c>
-      <c r="S44" s="2">
-        <f t="shared" si="0"/>
-        <v>29988.050000000003</v>
-      </c>
-    </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>37955</v>
       </c>
@@ -3181,12 +3001,8 @@
       <c r="R45">
         <v>97.65</v>
       </c>
-      <c r="S45" s="2">
-        <f t="shared" si="0"/>
-        <v>33766.31</v>
-      </c>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>38321</v>
       </c>
@@ -3241,12 +3057,8 @@
       <c r="R46">
         <v>115.04</v>
       </c>
-      <c r="S46" s="2">
-        <f t="shared" si="0"/>
-        <v>37853.609999999993</v>
-      </c>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>38686</v>
       </c>
@@ -3301,12 +3113,8 @@
       <c r="R47">
         <v>127.81</v>
       </c>
-      <c r="S47" s="2">
-        <f t="shared" si="0"/>
-        <v>40525.249999999993</v>
-      </c>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>39051</v>
       </c>
@@ -3361,12 +3169,8 @@
       <c r="R48">
         <v>148.63</v>
       </c>
-      <c r="S48" s="2">
-        <f t="shared" si="0"/>
-        <v>43487.83</v>
-      </c>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>39416</v>
       </c>
@@ -3421,12 +3225,8 @@
       <c r="R49">
         <v>180.94</v>
       </c>
-      <c r="S49" s="2">
-        <f t="shared" si="0"/>
-        <v>48625.890000000007</v>
-      </c>
-    </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>39782</v>
       </c>
@@ -3481,12 +3281,8 @@
       <c r="R50">
         <v>193.61</v>
       </c>
-      <c r="S50" s="2">
-        <f t="shared" si="0"/>
-        <v>52668.12</v>
-      </c>
-    </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>40147</v>
       </c>
@@ -3541,12 +3337,8 @@
       <c r="R51">
         <v>194.15</v>
       </c>
-      <c r="S51" s="2">
-        <f t="shared" si="0"/>
-        <v>50379.27</v>
-      </c>
-    </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>40512</v>
       </c>
@@ -3601,12 +3393,8 @@
       <c r="R52">
         <v>239.81</v>
       </c>
-      <c r="S52" s="2">
-        <f t="shared" si="0"/>
-        <v>54562.299999999988</v>
-      </c>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>40877</v>
       </c>
@@ -3661,12 +3449,8 @@
       <c r="R53">
         <v>279.35000000000002</v>
       </c>
-      <c r="S53" s="2">
-        <f t="shared" si="0"/>
-        <v>60339.729999999996</v>
-      </c>
-    </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>41243</v>
       </c>
@@ -3721,12 +3505,8 @@
       <c r="R54">
         <v>295.08999999999997</v>
       </c>
-      <c r="S54" s="2">
-        <f t="shared" si="0"/>
-        <v>61343.630000000005</v>
-      </c>
-    </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>41608</v>
       </c>
@@ -3781,12 +3561,8 @@
       <c r="R55">
         <v>307.58</v>
       </c>
-      <c r="S55" s="2">
-        <f t="shared" si="0"/>
-        <v>62955.05999999999</v>
-      </c>
-    </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>41973</v>
       </c>
@@ -3841,12 +3617,8 @@
       <c r="R56">
         <v>314.85000000000002</v>
       </c>
-      <c r="S56" s="2">
-        <f t="shared" si="0"/>
-        <v>64725.419999999984</v>
-      </c>
-    </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>42338</v>
       </c>
@@ -3901,12 +3673,8 @@
       <c r="R57">
         <v>308</v>
       </c>
-      <c r="S57" s="2">
-        <f t="shared" si="0"/>
-        <v>61614.05</v>
-      </c>
-    </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>42704</v>
       </c>
@@ -3961,12 +3729,8 @@
       <c r="R58">
         <v>318.76</v>
       </c>
-      <c r="S58" s="2">
-        <f t="shared" si="0"/>
-        <v>62942.720000000001</v>
-      </c>
-    </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>43069</v>
       </c>
@@ -4021,12 +3785,8 @@
       <c r="R59">
         <v>343.34</v>
       </c>
-      <c r="S59" s="2">
-        <f t="shared" si="0"/>
-        <v>66844.97</v>
-      </c>
-    </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>43434</v>
       </c>
@@ -4081,12 +3841,8 @@
       <c r="R60">
         <v>375.98</v>
       </c>
-      <c r="S60" s="2">
-        <f t="shared" si="0"/>
-        <v>71172.77</v>
-      </c>
-    </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>43799</v>
       </c>
@@ -4141,12 +3897,8 @@
       <c r="R61">
         <v>374.39</v>
       </c>
-      <c r="S61" s="2">
-        <f t="shared" si="0"/>
-        <v>72246.23</v>
-      </c>
-    </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>44165</v>
       </c>
@@ -4200,87 +3952,6 @@
       </c>
       <c r="R62" s="5">
         <v>340</v>
-      </c>
-      <c r="S62" s="2">
-        <f t="shared" si="0"/>
-        <v>70284.530000000013</v>
-      </c>
-    </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A63" s="1">
-        <v>44165</v>
-      </c>
-      <c r="B63" s="6">
-        <f>B62/(S62)</f>
-        <v>0.29788347450000724</v>
-      </c>
-      <c r="C63" s="6">
-        <f>C62/(S62)</f>
-        <v>0.20947326531172644</v>
-      </c>
-      <c r="D63" s="6">
-        <f>D62/(S62)</f>
-        <v>0.18511911511679735</v>
-      </c>
-      <c r="E63" s="6">
-        <f>E62/(S62)</f>
-        <v>7.0789688712437848E-2</v>
-      </c>
-      <c r="F63" s="6">
-        <f>F62/(S62)</f>
-        <v>3.8525405234978438E-2</v>
-      </c>
-      <c r="G63" s="6">
-        <f>G62/(S62)</f>
-        <v>3.7319449955772625E-2</v>
-      </c>
-      <c r="H63" s="6">
-        <f>H62/(S62)</f>
-        <v>2.3391207140461771E-2</v>
-      </c>
-      <c r="I63" s="6">
-        <f>I62/(S62)</f>
-        <v>2.319898845450058E-2</v>
-      </c>
-      <c r="J63" s="6">
-        <f>J62/(S62)</f>
-        <v>2.1107062962503979E-2</v>
-      </c>
-      <c r="K63" s="6">
-        <f>K62/(S62)</f>
-        <v>2.0555447976958796E-2</v>
-      </c>
-      <c r="L63" s="6">
-        <f>L62/(S62)</f>
-        <v>1.8935888167709164E-2</v>
-      </c>
-      <c r="M63" s="6">
-        <f>M62/(S62)</f>
-        <v>1.505907487750149E-2</v>
-      </c>
-      <c r="N63" s="6">
-        <f>N62/(S62)</f>
-        <v>1.0702924242361724E-2</v>
-      </c>
-      <c r="O63" s="6">
-        <f>O62/(S62)</f>
-        <v>1.0245497835725726E-2</v>
-      </c>
-      <c r="P63" s="6">
-        <f>P62/(S62)</f>
-        <v>7.6981378405745881E-3</v>
-      </c>
-      <c r="Q63" s="6">
-        <f>Q62/S62</f>
-        <v>5.1578917864286769E-3</v>
-      </c>
-      <c r="R63" s="6">
-        <f>R62/(S62)</f>
-        <v>4.8374798835533212E-3</v>
-      </c>
-      <c r="S63" s="7">
-        <f t="shared" si="0"/>
-        <v>0.99999999999999978</v>
       </c>
     </row>
   </sheetData>

</xml_diff>